<commit_message>
complete testing of querydb method.
</commit_message>
<xml_diff>
--- a/src/resources/emplid_license_request.xlsx
+++ b/src/resources/emplid_license_request.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nm150286\Documents\Projects\Professional_License_Lookup\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE4500E2-9386-4821-8548-2FDFC662A5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEF56C3-D108-4D3E-9E88-F28D7836222C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26925" yWindow="-13215" windowWidth="26055" windowHeight="28380" xr2:uid="{989CE8B9-C6FF-44D8-AA56-14B9E17A6AEC}"/>
+    <workbookView xWindow="-29070" yWindow="6870" windowWidth="26055" windowHeight="22560" xr2:uid="{989CE8B9-C6FF-44D8-AA56-14B9E17A6AEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Search_Request" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>123456</v>
+        <v>150286</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -441,7 +441,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>555555</v>
+        <v>150286</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>919191</v>
+        <v>122075</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -457,7 +457,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>991199</v>
+        <v>108054</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>

</xml_diff>